<commit_message>
Upload New Update in github
</commit_message>
<xml_diff>
--- a/FileCalcule.xlsx
+++ b/FileCalcule.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="117">
   <si>
     <t xml:space="preserve">*الملاحظات </t>
   </si>
@@ -530,34 +530,22 @@
     <t>ولاية الشلف</t>
   </si>
   <si>
-    <t>13/02/2020</t>
+    <t>04/11/2019</t>
   </si>
   <si>
     <t>06:00</t>
   </si>
   <si>
-    <t>20/02/2020</t>
-  </si>
-  <si>
-    <t>23:00</t>
-  </si>
-  <si>
-    <t>522</t>
-  </si>
-  <si>
-    <t>ولاية الأغواط</t>
-  </si>
-  <si>
-    <t>27/01/2020</t>
-  </si>
-  <si>
-    <t>30/01/2020</t>
-  </si>
-  <si>
-    <t>1000</t>
-  </si>
-  <si>
-    <t>2020/02/16</t>
+    <t>06/11/2019</t>
+  </si>
+  <si>
+    <t>255</t>
+  </si>
+  <si>
+    <t>متكفل بها</t>
+  </si>
+  <si>
+    <t>2021/07/19</t>
   </si>
 </sst>
 </file>
@@ -2635,21 +2623,23 @@
         <v>56</v>
       </c>
       <c r="L18" s="88"/>
-      <c r="N18" s="122">
-        <f>PRODUCT(O18:P18)</f>
+      <c r="N18" s="122" t="n">
+        <v>400.0</v>
       </c>
       <c r="O18" s="124" t="n">
         <v>400.0</v>
       </c>
       <c r="P18" s="101" t="n">
-        <v>16.0</v>
+        <v>4.0</v>
       </c>
       <c r="Q18" s="101"/>
       <c r="R18" s="101"/>
       <c r="S18" s="101" t="s">
         <v>91</v>
       </c>
-      <c r="U18" s="126"/>
+      <c r="U18" s="126" t="s">
+        <v>115</v>
+      </c>
       <c r="V18" s="125" t="s">
         <v>57</v>
       </c>
@@ -2675,14 +2665,14 @@
       <c r="J19" s="178"/>
       <c r="K19" s="82"/>
       <c r="L19" s="88"/>
-      <c r="N19" s="122">
-        <f>PRODUCT(O19:P19)</f>
+      <c r="N19" s="122" t="n">
+        <v>600.0</v>
       </c>
       <c r="O19" s="124" t="n">
         <v>1200.0</v>
       </c>
       <c r="P19" s="101" t="n">
-        <v>7.0</v>
+        <v>2.0</v>
       </c>
       <c r="Q19" s="101"/>
       <c r="R19" s="101"/>
@@ -2690,7 +2680,9 @@
         <v>92</v>
       </c>
       <c r="T19" s="125"/>
-      <c r="U19" s="126"/>
+      <c r="U19" s="126" t="s">
+        <v>115</v>
+      </c>
       <c r="V19" s="133" t="s">
         <v>60</v>
       </c>
@@ -2708,15 +2700,9 @@
       <c r="J20" s="178"/>
       <c r="K20" s="90"/>
       <c r="L20" s="88"/>
-      <c r="N20" s="122">
-        <f>PRODUCT(O20:P20)</f>
-      </c>
-      <c r="O20" s="124" t="n">
-        <v>500.0</v>
-      </c>
-      <c r="P20" s="101" t="n">
-        <v>8.0</v>
-      </c>
+      <c r="N20" s="122"/>
+      <c r="O20" s="124"/>
+      <c r="P20" s="101"/>
       <c r="Q20" s="101"/>
       <c r="R20" s="101"/>
       <c r="S20" s="101" t="s">
@@ -2740,15 +2726,9 @@
       <c r="J21" s="89"/>
       <c r="K21" s="90"/>
       <c r="L21" s="88"/>
-      <c r="N21" s="122">
-        <f>PRODUCT(O21:P21)</f>
-      </c>
-      <c r="O21" s="124" t="n">
-        <v>1500.0</v>
-      </c>
-      <c r="P21" s="101" t="n">
-        <v>3.0</v>
-      </c>
+      <c r="N21" s="122"/>
+      <c r="O21" s="124"/>
+      <c r="P21" s="101"/>
       <c r="Q21" s="101"/>
       <c r="R21" s="101"/>
       <c r="S21" s="101" t="s">
@@ -2796,7 +2776,7 @@
       <c r="J23" s="89"/>
       <c r="K23" s="90"/>
       <c r="N23" s="122">
-        <f>SUM(N18:N22)</f>
+        <f>SUM(N18:N19)</f>
       </c>
       <c r="O23" s="104" t="s">
         <v>65</v>
@@ -2837,7 +2817,7 @@
       <c r="K25" s="90"/>
       <c r="L25" s="88"/>
       <c r="N25" s="122" t="n">
-        <v>23300.0</v>
+        <v>1000.0</v>
       </c>
       <c r="O25" s="84" t="s">
         <v>68</v>
@@ -3078,7 +3058,7 @@
       <c r="I38" s="3"/>
       <c r="J38" s="3"/>
       <c r="L38" s="135" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="M38" s="135"/>
       <c r="N38" s="136" t="s">
@@ -3508,15 +3488,15 @@
     <row r="9" spans="1:21" ht="15.75" customHeight="1">
       <c r="A9" s="26"/>
       <c r="B9" s="128" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C9" s="108"/>
       <c r="D9" s="108" t="n">
-        <v>7.0</v>
+        <v>2.0</v>
       </c>
       <c r="E9" s="108"/>
       <c r="F9" s="109" t="n">
-        <v>16.0</v>
+        <v>4.0</v>
       </c>
       <c r="G9" s="27"/>
       <c r="H9" s="27"/>
@@ -3527,7 +3507,7 @@
         <v>109</v>
       </c>
       <c r="M9" s="116" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="N9" s="117" t="s">
         <v>113</v>
@@ -3552,47 +3532,27 @@
     <row r="10" spans="1:21" ht="16.5" customHeight="1">
       <c r="A10" s="28"/>
       <c r="B10" s="32" t="s">
-        <v>119</v>
-      </c>
-      <c r="C10" s="110" t="n">
-        <v>3.0</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="C10" s="110"/>
       <c r="D10" s="110"/>
-      <c r="E10" s="110" t="n">
-        <v>8.0</v>
-      </c>
+      <c r="E10" s="110"/>
       <c r="F10" s="111"/>
       <c r="G10" s="16"/>
       <c r="H10" s="16"/>
       <c r="I10" s="16"/>
       <c r="J10" s="29"/>
-      <c r="L10" s="64" t="s">
-        <v>109</v>
-      </c>
-      <c r="M10" s="64" t="s">
-        <v>114</v>
-      </c>
-      <c r="N10" s="76" t="s">
-        <v>118</v>
-      </c>
-      <c r="O10" s="64" t="s">
-        <v>112</v>
-      </c>
-      <c r="P10" s="75" t="s">
-        <v>117</v>
-      </c>
+      <c r="L10" s="64"/>
+      <c r="M10" s="64"/>
+      <c r="N10" s="76"/>
+      <c r="O10" s="64"/>
+      <c r="P10" s="75"/>
       <c r="Q10" s="68" t="s">
         <v>90</v>
       </c>
-      <c r="R10" s="69" t="s">
-        <v>116</v>
-      </c>
-      <c r="S10" s="70" t="s">
-        <v>107</v>
-      </c>
-      <c r="T10" s="64" t="s">
-        <v>109</v>
-      </c>
+      <c r="R10" s="69"/>
+      <c r="S10" s="70"/>
+      <c r="T10" s="64"/>
     </row>
     <row r="11" spans="1:21" ht="18.75">
       <c r="A11" s="28"/>

</xml_diff>